<commit_message>
Add email to fake users
</commit_message>
<xml_diff>
--- a/spec/fixtures/mock-data/FakeUsers.xlsx
+++ b/spec/fixtures/mock-data/FakeUsers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/src/osumb/challenges/spec/fixtures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/src/osumb/challenges/spec/fixtures/mock-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1638" uniqueCount="722">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1871" uniqueCount="722">
   <si>
     <t>Spot</t>
   </si>
@@ -2126,12 +2126,6 @@
     <t>Member</t>
   </si>
   <si>
-    <t>ApproveInstrument</t>
-  </si>
-  <si>
-    <t>ApprovePart</t>
-  </si>
-  <si>
     <t>Any</t>
   </si>
   <si>
@@ -2190,13 +2184,19 @@
   </si>
   <si>
     <t>Riber.8</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>tareshawty.3@osu.edu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2213,6 +2213,14 @@
       <color rgb="FF353535"/>
       <name val="PT Sans"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2300,10 +2308,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2320,8 +2329,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -2618,10 +2629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I235"/>
+  <dimension ref="A1:H235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A203" workbookViewId="0">
-      <selection activeCell="I235" sqref="I235"/>
+    <sheetView tabSelected="1" topLeftCell="A205" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2633,11 +2644,10 @@
     <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2660,13 +2670,10 @@
         <v>695</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>700</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>701</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -2683,13 +2690,16 @@
         <v>467</v>
       </c>
       <c r="F2" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="H2" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
@@ -2711,8 +2721,11 @@
       <c r="G3" s="4" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="H3" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -2734,8 +2747,11 @@
       <c r="G4" s="4" t="s">
         <v>477</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="H4" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
@@ -2757,8 +2773,11 @@
       <c r="G5" s="4" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="H5" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>473</v>
       </c>
@@ -2780,8 +2799,11 @@
       <c r="G6" s="4" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="H6" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
@@ -2803,8 +2825,11 @@
       <c r="G7" s="4" t="s">
         <v>479</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="H7" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
@@ -2826,8 +2851,11 @@
       <c r="G8" s="4" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="H8" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
@@ -2849,8 +2877,11 @@
       <c r="G9" s="4" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="H9" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>14</v>
       </c>
@@ -2872,8 +2903,11 @@
       <c r="G10" s="4" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="H10" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
@@ -2895,8 +2929,11 @@
       <c r="G11" s="4" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="H11" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
@@ -2918,8 +2955,11 @@
       <c r="G12" s="4" t="s">
         <v>484</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="H12" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
@@ -2936,13 +2976,16 @@
         <v>485</v>
       </c>
       <c r="F13" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>485</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="H13" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
@@ -2964,8 +3007,11 @@
       <c r="G14" s="4" t="s">
         <v>486</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="H14" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>19</v>
       </c>
@@ -2987,8 +3033,11 @@
       <c r="G15" s="4" t="s">
         <v>487</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="H15" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>20</v>
       </c>
@@ -3005,13 +3054,16 @@
         <v>488</v>
       </c>
       <c r="F16" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H16" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>22</v>
       </c>
@@ -3033,8 +3085,11 @@
       <c r="G17" s="4" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H17" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>24</v>
       </c>
@@ -3056,8 +3111,11 @@
       <c r="G18" s="4" t="s">
         <v>490</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H18" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>25</v>
       </c>
@@ -3079,8 +3137,11 @@
       <c r="G19" s="4" t="s">
         <v>491</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H19" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>26</v>
       </c>
@@ -3102,8 +3163,11 @@
       <c r="G20" s="4" t="s">
         <v>492</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H20" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>27</v>
       </c>
@@ -3125,8 +3189,11 @@
       <c r="G21" s="4" t="s">
         <v>493</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H21" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>28</v>
       </c>
@@ -3148,8 +3215,11 @@
       <c r="G22" s="4" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H22" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>29</v>
       </c>
@@ -3171,8 +3241,11 @@
       <c r="G23" s="4" t="s">
         <v>495</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H23" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>30</v>
       </c>
@@ -3194,8 +3267,11 @@
       <c r="G24" s="4" t="s">
         <v>496</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H24" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>31</v>
       </c>
@@ -3217,8 +3293,11 @@
       <c r="G25" s="4" t="s">
         <v>497</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H25" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>32</v>
       </c>
@@ -3240,8 +3319,11 @@
       <c r="G26" s="4" t="s">
         <v>498</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H26" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>33</v>
       </c>
@@ -3258,13 +3340,16 @@
         <v>499</v>
       </c>
       <c r="F27" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H27" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>34</v>
       </c>
@@ -3286,8 +3371,11 @@
       <c r="G28" s="4" t="s">
         <v>500</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H28" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>35</v>
       </c>
@@ -3309,8 +3397,11 @@
       <c r="G29" s="4" t="s">
         <v>501</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H29" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>36</v>
       </c>
@@ -3327,13 +3418,16 @@
         <v>502</v>
       </c>
       <c r="F30" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H30" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>38</v>
       </c>
@@ -3355,8 +3449,11 @@
       <c r="G31" s="4" t="s">
         <v>503</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H31" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>39</v>
       </c>
@@ -3378,8 +3475,11 @@
       <c r="G32" s="4" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H32" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>40</v>
       </c>
@@ -3401,8 +3501,11 @@
       <c r="G33" s="4" t="s">
         <v>505</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H33" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>41</v>
       </c>
@@ -3424,8 +3527,11 @@
       <c r="G34" s="4" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H34" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>42</v>
       </c>
@@ -3447,8 +3553,11 @@
       <c r="G35" s="4" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H35" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>43</v>
       </c>
@@ -3470,8 +3579,11 @@
       <c r="G36" s="4" t="s">
         <v>508</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H36" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>44</v>
       </c>
@@ -3493,8 +3605,11 @@
       <c r="G37" s="4" t="s">
         <v>509</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H37" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>45</v>
       </c>
@@ -3516,8 +3631,11 @@
       <c r="G38" s="4" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H38" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>46</v>
       </c>
@@ -3539,8 +3657,11 @@
       <c r="G39" s="4" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H39" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>47</v>
       </c>
@@ -3562,8 +3683,11 @@
       <c r="G40" s="4" t="s">
         <v>468</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H40" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>48</v>
       </c>
@@ -3580,13 +3704,16 @@
         <v>512</v>
       </c>
       <c r="F41" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="G41" s="4" t="s">
         <v>512</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H41" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>49</v>
       </c>
@@ -3608,8 +3735,11 @@
       <c r="G42" s="4" t="s">
         <v>513</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H42" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>50</v>
       </c>
@@ -3631,8 +3761,11 @@
       <c r="G43" s="4" t="s">
         <v>514</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H43" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>51</v>
       </c>
@@ -3649,13 +3782,16 @@
         <v>515</v>
       </c>
       <c r="F44" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>515</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H44" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>53</v>
       </c>
@@ -3677,8 +3813,11 @@
       <c r="G45" s="4" t="s">
         <v>516</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H45" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>54</v>
       </c>
@@ -3700,8 +3839,11 @@
       <c r="G46" s="4" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H46" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>55</v>
       </c>
@@ -3723,8 +3865,11 @@
       <c r="G47" s="4" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H47" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>56</v>
       </c>
@@ -3746,8 +3891,11 @@
       <c r="G48" s="4" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H48" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>57</v>
       </c>
@@ -3769,8 +3917,11 @@
       <c r="G49" s="4" t="s">
         <v>520</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H49" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>58</v>
       </c>
@@ -3792,8 +3943,11 @@
       <c r="G50" s="4" t="s">
         <v>521</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H50" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>59</v>
       </c>
@@ -3815,8 +3969,11 @@
       <c r="G51" s="4" t="s">
         <v>522</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H51" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>60</v>
       </c>
@@ -3838,8 +3995,11 @@
       <c r="G52" s="4" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H52" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>61</v>
       </c>
@@ -3861,8 +4021,11 @@
       <c r="G53" s="4" t="s">
         <v>524</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H53" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>62</v>
       </c>
@@ -3884,8 +4047,11 @@
       <c r="G54" s="4" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H54" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>63</v>
       </c>
@@ -3902,13 +4068,16 @@
         <v>526</v>
       </c>
       <c r="F55" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="G55" s="4" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H55" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>64</v>
       </c>
@@ -3930,8 +4099,11 @@
       <c r="G56" s="4" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H56" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>65</v>
       </c>
@@ -3953,8 +4125,11 @@
       <c r="G57" s="4" t="s">
         <v>528</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H57" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>66</v>
       </c>
@@ -3971,13 +4146,16 @@
         <v>529</v>
       </c>
       <c r="F58" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="G58" s="4" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H58" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>69</v>
       </c>
@@ -3999,8 +4177,11 @@
       <c r="G59" s="4" t="s">
         <v>530</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H59" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>70</v>
       </c>
@@ -4022,8 +4203,11 @@
       <c r="G60" s="4" t="s">
         <v>531</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H60" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>71</v>
       </c>
@@ -4045,8 +4229,11 @@
       <c r="G61" s="4" t="s">
         <v>532</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H61" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>72</v>
       </c>
@@ -4068,8 +4255,11 @@
       <c r="G62" s="4" t="s">
         <v>533</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H62" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>73</v>
       </c>
@@ -4091,8 +4281,11 @@
       <c r="G63" s="4" t="s">
         <v>534</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H63" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>234</v>
       </c>
@@ -4114,8 +4307,11 @@
       <c r="G64" s="4" t="s">
         <v>535</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H64" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>74</v>
       </c>
@@ -4137,8 +4333,11 @@
       <c r="G65" s="4" t="s">
         <v>536</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H65" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>75</v>
       </c>
@@ -4160,8 +4359,11 @@
       <c r="G66" s="4" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H66" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>76</v>
       </c>
@@ -4183,8 +4385,11 @@
       <c r="G67" s="4" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H67" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>77</v>
       </c>
@@ -4206,8 +4411,11 @@
       <c r="G68" s="4" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H68" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>78</v>
       </c>
@@ -4224,13 +4432,16 @@
         <v>540</v>
       </c>
       <c r="F69" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="G69" s="4" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H69" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>79</v>
       </c>
@@ -4252,8 +4463,11 @@
       <c r="G70" s="4" t="s">
         <v>541</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H70" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
         <v>80</v>
       </c>
@@ -4275,8 +4489,11 @@
       <c r="G71" s="4" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H71" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
         <v>235</v>
       </c>
@@ -4293,13 +4510,16 @@
         <v>543</v>
       </c>
       <c r="F72" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="G72" s="4" t="s">
         <v>543</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H72" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
         <v>81</v>
       </c>
@@ -4321,8 +4541,11 @@
       <c r="G73" s="4" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H73" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>83</v>
       </c>
@@ -4344,8 +4567,11 @@
       <c r="G74" s="4" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H74" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>84</v>
       </c>
@@ -4367,8 +4593,11 @@
       <c r="G75" s="4" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H75" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>85</v>
       </c>
@@ -4390,8 +4619,11 @@
       <c r="G76" s="4" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H76" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>86</v>
       </c>
@@ -4413,8 +4645,11 @@
       <c r="G77" s="4" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H77" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>87</v>
       </c>
@@ -4436,8 +4671,11 @@
       <c r="G78" s="4" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H78" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>88</v>
       </c>
@@ -4459,8 +4697,11 @@
       <c r="G79" s="4" t="s">
         <v>550</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H79" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>89</v>
       </c>
@@ -4482,8 +4723,11 @@
       <c r="G80" s="4" t="s">
         <v>469</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H80" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>90</v>
       </c>
@@ -4505,8 +4749,11 @@
       <c r="G81" s="4" t="s">
         <v>551</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H81" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>91</v>
       </c>
@@ -4528,8 +4775,11 @@
       <c r="G82" s="4" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H82" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>92</v>
       </c>
@@ -4546,13 +4796,16 @@
         <v>553</v>
       </c>
       <c r="F83" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="G83" s="4" t="s">
         <v>553</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H83" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>93</v>
       </c>
@@ -4574,8 +4827,11 @@
       <c r="G84" s="4" t="s">
         <v>554</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H84" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
         <v>94</v>
       </c>
@@ -4597,8 +4853,11 @@
       <c r="G85" s="4" t="s">
         <v>555</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H85" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>95</v>
       </c>
@@ -4606,7 +4865,7 @@
         <v>328</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D86" s="6" t="s">
         <v>96</v>
@@ -4620,8 +4879,11 @@
       <c r="G86" s="4" t="s">
         <v>556</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H86" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>97</v>
       </c>
@@ -4629,7 +4891,7 @@
         <v>329</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D87" s="6" t="s">
         <v>96</v>
@@ -4643,8 +4905,11 @@
       <c r="G87" s="4" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H87" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>98</v>
       </c>
@@ -4652,7 +4917,7 @@
         <v>330</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D88" s="6" t="s">
         <v>96</v>
@@ -4666,8 +4931,11 @@
       <c r="G88" s="4" t="s">
         <v>558</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H88" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>99</v>
       </c>
@@ -4675,7 +4943,7 @@
         <v>331</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D89" s="6" t="s">
         <v>96</v>
@@ -4689,8 +4957,11 @@
       <c r="G89" s="4" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H89" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>100</v>
       </c>
@@ -4698,7 +4969,7 @@
         <v>332</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D90" s="6" t="s">
         <v>96</v>
@@ -4712,8 +4983,11 @@
       <c r="G90" s="4" t="s">
         <v>560</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H90" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>101</v>
       </c>
@@ -4721,7 +4995,7 @@
         <v>333</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D91" s="6" t="s">
         <v>96</v>
@@ -4730,13 +5004,16 @@
         <v>561</v>
       </c>
       <c r="F91" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="G91" s="4" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H91" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>102</v>
       </c>
@@ -4744,7 +5021,7 @@
         <v>334</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D92" s="6" t="s">
         <v>96</v>
@@ -4758,8 +5035,11 @@
       <c r="G92" s="4" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H92" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>103</v>
       </c>
@@ -4767,7 +5047,7 @@
         <v>335</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D93" s="6" t="s">
         <v>96</v>
@@ -4781,8 +5061,11 @@
       <c r="G93" s="4" t="s">
         <v>563</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H93" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
         <v>104</v>
       </c>
@@ -4790,7 +5073,7 @@
         <v>336</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D94" s="6" t="s">
         <v>96</v>
@@ -4804,8 +5087,11 @@
       <c r="G94" s="4" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H94" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
         <v>105</v>
       </c>
@@ -4813,7 +5099,7 @@
         <v>337</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D95" s="6" t="s">
         <v>96</v>
@@ -4827,8 +5113,11 @@
       <c r="G95" s="4" t="s">
         <v>565</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H95" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
         <v>106</v>
       </c>
@@ -4836,7 +5125,7 @@
         <v>338</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D96" s="6" t="s">
         <v>96</v>
@@ -4850,8 +5139,11 @@
       <c r="G96" s="4" t="s">
         <v>566</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H96" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
         <v>107</v>
       </c>
@@ -4859,7 +5151,7 @@
         <v>339</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D97" s="6" t="s">
         <v>96</v>
@@ -4868,13 +5160,16 @@
         <v>567</v>
       </c>
       <c r="F97" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="G97" s="4" t="s">
         <v>567</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H97" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
         <v>236</v>
       </c>
@@ -4882,7 +5177,7 @@
         <v>340</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D98" s="6" t="s">
         <v>96</v>
@@ -4896,8 +5191,11 @@
       <c r="G98" s="4" t="s">
         <v>568</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H98" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
         <v>108</v>
       </c>
@@ -4905,7 +5203,7 @@
         <v>341</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D99" s="6" t="s">
         <v>96</v>
@@ -4919,8 +5217,11 @@
       <c r="G99" s="4" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H99" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>109</v>
       </c>
@@ -4928,7 +5229,7 @@
         <v>342</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D100" s="6" t="s">
         <v>110</v>
@@ -4937,13 +5238,16 @@
         <v>570</v>
       </c>
       <c r="F100" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="G100" s="4" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H100" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>237</v>
       </c>
@@ -4951,7 +5255,7 @@
         <v>343</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D101" s="6" t="s">
         <v>68</v>
@@ -4965,8 +5269,11 @@
       <c r="G101" s="4" t="s">
         <v>571</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H101" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
         <v>111</v>
       </c>
@@ -4974,7 +5281,7 @@
         <v>344</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D102" s="6" t="s">
         <v>68</v>
@@ -4983,13 +5290,16 @@
         <v>572</v>
       </c>
       <c r="F102" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="G102" s="4" t="s">
         <v>572</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H102" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
         <v>112</v>
       </c>
@@ -4997,7 +5307,7 @@
         <v>242</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D103" s="6" t="s">
         <v>113</v>
@@ -5011,8 +5321,11 @@
       <c r="G103" s="4" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H103" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
         <v>114</v>
       </c>
@@ -5020,7 +5333,7 @@
         <v>345</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D104" s="6" t="s">
         <v>113</v>
@@ -5029,13 +5342,16 @@
         <v>574</v>
       </c>
       <c r="F104" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="G104" s="4" t="s">
         <v>574</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H104" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
         <v>115</v>
       </c>
@@ -5043,7 +5359,7 @@
         <v>346</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D105" s="6" t="s">
         <v>68</v>
@@ -5057,8 +5373,11 @@
       <c r="G105" s="4" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H105" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
         <v>116</v>
       </c>
@@ -5066,7 +5385,7 @@
         <v>347</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D106" s="6" t="s">
         <v>68</v>
@@ -5080,8 +5399,11 @@
       <c r="G106" s="4" t="s">
         <v>576</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H106" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
         <v>117</v>
       </c>
@@ -5089,7 +5411,7 @@
         <v>348</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D107" s="6" t="s">
         <v>113</v>
@@ -5103,8 +5425,11 @@
       <c r="G107" s="4" t="s">
         <v>577</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H107" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
         <v>118</v>
       </c>
@@ -5112,7 +5437,7 @@
         <v>349</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D108" s="6" t="s">
         <v>113</v>
@@ -5126,8 +5451,11 @@
       <c r="G108" s="4" t="s">
         <v>578</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H108" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
         <v>119</v>
       </c>
@@ -5135,7 +5463,7 @@
         <v>350</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D109" s="6" t="s">
         <v>68</v>
@@ -5149,8 +5477,11 @@
       <c r="G109" s="4" t="s">
         <v>579</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H109" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
         <v>120</v>
       </c>
@@ -5158,7 +5489,7 @@
         <v>351</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D110" s="6" t="s">
         <v>110</v>
@@ -5172,8 +5503,11 @@
       <c r="G110" s="4" t="s">
         <v>580</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H110" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
         <v>121</v>
       </c>
@@ -5181,7 +5515,7 @@
         <v>352</v>
       </c>
       <c r="C111" s="6" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D111" s="6" t="s">
         <v>110</v>
@@ -5195,8 +5529,11 @@
       <c r="G111" s="4" t="s">
         <v>581</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H111" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
         <v>122</v>
       </c>
@@ -5204,7 +5541,7 @@
         <v>353</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D112" s="6" t="s">
         <v>110</v>
@@ -5218,8 +5555,11 @@
       <c r="G112" s="4" t="s">
         <v>582</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H112" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
         <v>123</v>
       </c>
@@ -5227,7 +5567,7 @@
         <v>354</v>
       </c>
       <c r="C113" s="6" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D113" s="6" t="s">
         <v>68</v>
@@ -5241,8 +5581,11 @@
       <c r="G113" s="4" t="s">
         <v>583</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H113" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A114" s="7" t="s">
         <v>124</v>
       </c>
@@ -5250,7 +5593,7 @@
         <v>355</v>
       </c>
       <c r="C114" s="6" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D114" s="8" t="s">
         <v>113</v>
@@ -5264,8 +5607,11 @@
       <c r="G114" s="4" t="s">
         <v>584</v>
       </c>
-    </row>
-    <row r="115" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H114" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
         <v>125</v>
       </c>
@@ -5282,13 +5628,16 @@
         <v>585</v>
       </c>
       <c r="F115" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="G115" s="4" t="s">
         <v>585</v>
       </c>
-    </row>
-    <row r="116" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H115" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
         <v>127</v>
       </c>
@@ -5310,8 +5659,11 @@
       <c r="G116" s="4" t="s">
         <v>586</v>
       </c>
-    </row>
-    <row r="117" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H116" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
         <v>128</v>
       </c>
@@ -5333,8 +5685,11 @@
       <c r="G117" s="4" t="s">
         <v>587</v>
       </c>
-    </row>
-    <row r="118" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H117" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
         <v>238</v>
       </c>
@@ -5356,8 +5711,11 @@
       <c r="G118" s="4" t="s">
         <v>588</v>
       </c>
-    </row>
-    <row r="119" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H118" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
         <v>129</v>
       </c>
@@ -5379,8 +5737,11 @@
       <c r="G119" s="4" t="s">
         <v>589</v>
       </c>
-    </row>
-    <row r="120" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H119" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
         <v>130</v>
       </c>
@@ -5402,8 +5763,11 @@
       <c r="G120" s="4" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="121" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H120" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
         <v>131</v>
       </c>
@@ -5425,8 +5789,11 @@
       <c r="G121" s="4" t="s">
         <v>590</v>
       </c>
-    </row>
-    <row r="122" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H121" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
         <v>132</v>
       </c>
@@ -5448,8 +5815,11 @@
       <c r="G122" s="4" t="s">
         <v>591</v>
       </c>
-    </row>
-    <row r="123" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H122" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
         <v>133</v>
       </c>
@@ -5471,8 +5841,11 @@
       <c r="G123" s="4" t="s">
         <v>592</v>
       </c>
-    </row>
-    <row r="124" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H123" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
         <v>134</v>
       </c>
@@ -5494,8 +5867,11 @@
       <c r="G124" s="4" t="s">
         <v>593</v>
       </c>
-    </row>
-    <row r="125" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H124" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
         <v>135</v>
       </c>
@@ -5517,8 +5893,11 @@
       <c r="G125" s="4" t="s">
         <v>594</v>
       </c>
-    </row>
-    <row r="126" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H125" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
         <v>136</v>
       </c>
@@ -5535,13 +5914,16 @@
         <v>595</v>
       </c>
       <c r="F126" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="G126" s="4" t="s">
         <v>595</v>
       </c>
-    </row>
-    <row r="127" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H126" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
         <v>137</v>
       </c>
@@ -5563,8 +5945,11 @@
       <c r="G127" s="4" t="s">
         <v>596</v>
       </c>
-    </row>
-    <row r="128" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H127" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A128" s="7" t="s">
         <v>138</v>
       </c>
@@ -5586,8 +5971,11 @@
       <c r="G128" s="4" t="s">
         <v>597</v>
       </c>
-    </row>
-    <row r="129" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H128" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
         <v>139</v>
       </c>
@@ -5604,13 +5992,16 @@
         <v>598</v>
       </c>
       <c r="F129" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="G129" s="4" t="s">
         <v>598</v>
       </c>
-    </row>
-    <row r="130" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H129" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
         <v>140</v>
       </c>
@@ -5632,8 +6023,11 @@
       <c r="G130" s="4" t="s">
         <v>599</v>
       </c>
-    </row>
-    <row r="131" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H130" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
         <v>141</v>
       </c>
@@ -5655,8 +6049,11 @@
       <c r="G131" s="4" t="s">
         <v>600</v>
       </c>
-    </row>
-    <row r="132" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H131" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
         <v>240</v>
       </c>
@@ -5678,8 +6075,11 @@
       <c r="G132" s="4" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="133" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H132" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
         <v>142</v>
       </c>
@@ -5701,8 +6101,11 @@
       <c r="G133" s="4" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="134" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H133" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
         <v>143</v>
       </c>
@@ -5724,8 +6127,11 @@
       <c r="G134" s="4" t="s">
         <v>603</v>
       </c>
-    </row>
-    <row r="135" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H134" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
         <v>144</v>
       </c>
@@ -5747,8 +6153,11 @@
       <c r="G135" s="4" t="s">
         <v>604</v>
       </c>
-    </row>
-    <row r="136" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H135" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
         <v>145</v>
       </c>
@@ -5770,8 +6179,11 @@
       <c r="G136" s="4" t="s">
         <v>605</v>
       </c>
-    </row>
-    <row r="137" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H136" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
         <v>146</v>
       </c>
@@ -5793,8 +6205,11 @@
       <c r="G137" s="4" t="s">
         <v>606</v>
       </c>
-    </row>
-    <row r="138" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H137" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
         <v>147</v>
       </c>
@@ -5816,8 +6231,11 @@
       <c r="G138" s="4" t="s">
         <v>607</v>
       </c>
-    </row>
-    <row r="139" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H138" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
         <v>148</v>
       </c>
@@ -5839,8 +6257,11 @@
       <c r="G139" s="4" t="s">
         <v>608</v>
       </c>
-    </row>
-    <row r="140" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H139" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
         <v>149</v>
       </c>
@@ -5857,13 +6278,16 @@
         <v>609</v>
       </c>
       <c r="F140" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="G140" s="4" t="s">
         <v>609</v>
       </c>
-    </row>
-    <row r="141" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H140" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
         <v>150</v>
       </c>
@@ -5885,8 +6309,11 @@
       <c r="G141" s="4" t="s">
         <v>610</v>
       </c>
-    </row>
-    <row r="142" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H141" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
         <v>239</v>
       </c>
@@ -5908,8 +6335,11 @@
       <c r="G142" s="4" t="s">
         <v>611</v>
       </c>
-    </row>
-    <row r="143" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H142" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
         <v>151</v>
       </c>
@@ -5926,13 +6356,16 @@
         <v>612</v>
       </c>
       <c r="F143" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="G143" s="4" t="s">
         <v>612</v>
       </c>
-    </row>
-    <row r="144" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H143" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A144" s="5" t="s">
         <v>152</v>
       </c>
@@ -5954,8 +6387,11 @@
       <c r="G144" s="4" t="s">
         <v>613</v>
       </c>
-    </row>
-    <row r="145" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H144" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
         <v>153</v>
       </c>
@@ -5977,8 +6413,11 @@
       <c r="G145" s="4" t="s">
         <v>614</v>
       </c>
-    </row>
-    <row r="146" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H145" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
         <v>154</v>
       </c>
@@ -6000,8 +6439,11 @@
       <c r="G146" s="4" t="s">
         <v>615</v>
       </c>
-    </row>
-    <row r="147" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H146" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
         <v>155</v>
       </c>
@@ -6023,8 +6465,11 @@
       <c r="G147" s="4" t="s">
         <v>616</v>
       </c>
-    </row>
-    <row r="148" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H147" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
         <v>156</v>
       </c>
@@ -6046,8 +6491,11 @@
       <c r="G148" s="4" t="s">
         <v>617</v>
       </c>
-    </row>
-    <row r="149" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H148" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
         <v>157</v>
       </c>
@@ -6069,8 +6517,11 @@
       <c r="G149" s="4" t="s">
         <v>618</v>
       </c>
-    </row>
-    <row r="150" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H149" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
         <v>158</v>
       </c>
@@ -6092,8 +6543,11 @@
       <c r="G150" s="4" t="s">
         <v>619</v>
       </c>
-    </row>
-    <row r="151" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H150" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
         <v>159</v>
       </c>
@@ -6115,8 +6569,11 @@
       <c r="G151" s="4" t="s">
         <v>620</v>
       </c>
-    </row>
-    <row r="152" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H151" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
         <v>160</v>
       </c>
@@ -6138,8 +6595,11 @@
       <c r="G152" s="4" t="s">
         <v>621</v>
       </c>
-    </row>
-    <row r="153" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H152" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
         <v>161</v>
       </c>
@@ -6161,8 +6621,11 @@
       <c r="G153" s="4" t="s">
         <v>622</v>
       </c>
-    </row>
-    <row r="154" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H153" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
         <v>162</v>
       </c>
@@ -6179,13 +6642,16 @@
         <v>623</v>
       </c>
       <c r="F154" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="G154" s="4" t="s">
         <v>623</v>
       </c>
-    </row>
-    <row r="155" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H154" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
         <v>163</v>
       </c>
@@ -6207,8 +6673,11 @@
       <c r="G155" s="4" t="s">
         <v>624</v>
       </c>
-    </row>
-    <row r="156" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H155" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A156" s="7" t="s">
         <v>164</v>
       </c>
@@ -6230,8 +6699,11 @@
       <c r="G156" s="4" t="s">
         <v>625</v>
       </c>
-    </row>
-    <row r="157" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H156" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
         <v>165</v>
       </c>
@@ -6248,13 +6720,16 @@
         <v>626</v>
       </c>
       <c r="F157" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="G157" s="4" t="s">
         <v>626</v>
       </c>
-    </row>
-    <row r="158" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H157" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
         <v>166</v>
       </c>
@@ -6276,8 +6751,11 @@
       <c r="G158" s="4" t="s">
         <v>627</v>
       </c>
-    </row>
-    <row r="159" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H158" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
         <v>167</v>
       </c>
@@ -6299,8 +6777,11 @@
       <c r="G159" s="4" t="s">
         <v>628</v>
       </c>
-    </row>
-    <row r="160" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H159" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
         <v>168</v>
       </c>
@@ -6322,8 +6803,11 @@
       <c r="G160" s="4" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="161" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H160" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
         <v>169</v>
       </c>
@@ -6345,8 +6829,11 @@
       <c r="G161" s="4" t="s">
         <v>629</v>
       </c>
-    </row>
-    <row r="162" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H161" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
         <v>170</v>
       </c>
@@ -6368,8 +6855,11 @@
       <c r="G162" s="4" t="s">
         <v>630</v>
       </c>
-    </row>
-    <row r="163" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H162" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
         <v>171</v>
       </c>
@@ -6391,8 +6881,11 @@
       <c r="G163" s="4" t="s">
         <v>631</v>
       </c>
-    </row>
-    <row r="164" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H163" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
         <v>172</v>
       </c>
@@ -6414,8 +6907,11 @@
       <c r="G164" s="4" t="s">
         <v>632</v>
       </c>
-    </row>
-    <row r="165" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H164" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
         <v>241</v>
       </c>
@@ -6437,8 +6933,11 @@
       <c r="G165" s="4" t="s">
         <v>633</v>
       </c>
-    </row>
-    <row r="166" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H165" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
         <v>173</v>
       </c>
@@ -6460,8 +6959,11 @@
       <c r="G166" s="4" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="167" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H166" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
         <v>174</v>
       </c>
@@ -6483,8 +6985,11 @@
       <c r="G167" s="4" t="s">
         <v>635</v>
       </c>
-    </row>
-    <row r="168" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H167" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
         <v>175</v>
       </c>
@@ -6501,13 +7006,16 @@
         <v>636</v>
       </c>
       <c r="F168" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="G168" s="4" t="s">
         <v>636</v>
       </c>
-    </row>
-    <row r="169" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H168" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A169" s="5" t="s">
         <v>176</v>
       </c>
@@ -6529,8 +7037,11 @@
       <c r="G169" s="4" t="s">
         <v>637</v>
       </c>
-    </row>
-    <row r="170" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H169" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A170" s="7" t="s">
         <v>177</v>
       </c>
@@ -6552,8 +7063,11 @@
       <c r="G170" s="4" t="s">
         <v>638</v>
       </c>
-    </row>
-    <row r="171" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H170" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
         <v>178</v>
       </c>
@@ -6570,13 +7084,16 @@
         <v>639</v>
       </c>
       <c r="F171" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="G171" s="4" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="172" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H171" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A172" s="5" t="s">
         <v>179</v>
       </c>
@@ -6598,8 +7115,11 @@
       <c r="G172" s="4" t="s">
         <v>640</v>
       </c>
-    </row>
-    <row r="173" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H172" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A173" s="5" t="s">
         <v>180</v>
       </c>
@@ -6621,8 +7141,11 @@
       <c r="G173" s="4" t="s">
         <v>641</v>
       </c>
-    </row>
-    <row r="174" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H173" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A174" s="5" t="s">
         <v>181</v>
       </c>
@@ -6644,8 +7167,11 @@
       <c r="G174" s="4" t="s">
         <v>642</v>
       </c>
-    </row>
-    <row r="175" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H174" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A175" s="5" t="s">
         <v>182</v>
       </c>
@@ -6667,8 +7193,11 @@
       <c r="G175" s="4" t="s">
         <v>643</v>
       </c>
-    </row>
-    <row r="176" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H175" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A176" s="5" t="s">
         <v>183</v>
       </c>
@@ -6690,8 +7219,11 @@
       <c r="G176" s="4" t="s">
         <v>644</v>
       </c>
-    </row>
-    <row r="177" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H176" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A177" s="5" t="s">
         <v>184</v>
       </c>
@@ -6713,8 +7245,11 @@
       <c r="G177" s="4" t="s">
         <v>645</v>
       </c>
-    </row>
-    <row r="178" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H177" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A178" s="5" t="s">
         <v>185</v>
       </c>
@@ -6736,8 +7271,11 @@
       <c r="G178" s="4" t="s">
         <v>646</v>
       </c>
-    </row>
-    <row r="179" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H178" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A179" s="5" t="s">
         <v>186</v>
       </c>
@@ -6759,8 +7297,11 @@
       <c r="G179" s="4" t="s">
         <v>647</v>
       </c>
-    </row>
-    <row r="180" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H179" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A180" s="5" t="s">
         <v>187</v>
       </c>
@@ -6782,8 +7323,11 @@
       <c r="G180" s="4" t="s">
         <v>648</v>
       </c>
-    </row>
-    <row r="181" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H180" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A181" s="5" t="s">
         <v>188</v>
       </c>
@@ -6805,8 +7349,11 @@
       <c r="G181" s="4" t="s">
         <v>649</v>
       </c>
-    </row>
-    <row r="182" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H181" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A182" s="5" t="s">
         <v>189</v>
       </c>
@@ -6823,13 +7370,16 @@
         <v>650</v>
       </c>
       <c r="F182" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="G182" s="4" t="s">
         <v>650</v>
       </c>
-    </row>
-    <row r="183" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H182" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A183" s="5" t="s">
         <v>190</v>
       </c>
@@ -6851,8 +7401,11 @@
       <c r="G183" s="4" t="s">
         <v>651</v>
       </c>
-    </row>
-    <row r="184" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H183" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A184" s="7" t="s">
         <v>191</v>
       </c>
@@ -6874,8 +7427,11 @@
       <c r="G184" s="4" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="185" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H184" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A185" s="5" t="s">
         <v>192</v>
       </c>
@@ -6892,13 +7448,16 @@
         <v>653</v>
       </c>
       <c r="F185" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="G185" s="4" t="s">
         <v>653</v>
       </c>
-    </row>
-    <row r="186" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H185" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A186" s="5" t="s">
         <v>193</v>
       </c>
@@ -6920,8 +7479,11 @@
       <c r="G186" s="4" t="s">
         <v>654</v>
       </c>
-    </row>
-    <row r="187" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H186" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A187" s="5" t="s">
         <v>194</v>
       </c>
@@ -6943,8 +7505,11 @@
       <c r="G187" s="4" t="s">
         <v>655</v>
       </c>
-    </row>
-    <row r="188" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H187" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A188" s="5" t="s">
         <v>195</v>
       </c>
@@ -6966,8 +7531,11 @@
       <c r="G188" s="4" t="s">
         <v>656</v>
       </c>
-    </row>
-    <row r="189" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H188" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A189" s="5" t="s">
         <v>196</v>
       </c>
@@ -6989,8 +7557,11 @@
       <c r="G189" s="4" t="s">
         <v>657</v>
       </c>
-    </row>
-    <row r="190" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H189" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A190" s="5" t="s">
         <v>197</v>
       </c>
@@ -7012,8 +7583,11 @@
       <c r="G190" s="4" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="191" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H190" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A191" s="5" t="s">
         <v>198</v>
       </c>
@@ -7035,8 +7609,11 @@
       <c r="G191" s="4" t="s">
         <v>659</v>
       </c>
-    </row>
-    <row r="192" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H191" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A192" s="5" t="s">
         <v>199</v>
       </c>
@@ -7058,8 +7635,11 @@
       <c r="G192" s="4" t="s">
         <v>660</v>
       </c>
-    </row>
-    <row r="193" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H192" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A193" s="5" t="s">
         <v>200</v>
       </c>
@@ -7081,8 +7661,11 @@
       <c r="G193" s="4" t="s">
         <v>661</v>
       </c>
-    </row>
-    <row r="194" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H193" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A194" s="5" t="s">
         <v>201</v>
       </c>
@@ -7104,8 +7687,11 @@
       <c r="G194" s="4" t="s">
         <v>662</v>
       </c>
-    </row>
-    <row r="195" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H194" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A195" s="5" t="s">
         <v>202</v>
       </c>
@@ -7127,8 +7713,11 @@
       <c r="G195" s="4" t="s">
         <v>663</v>
       </c>
-    </row>
-    <row r="196" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H195" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A196" s="5" t="s">
         <v>203</v>
       </c>
@@ -7145,13 +7734,16 @@
         <v>664</v>
       </c>
       <c r="F196" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="G196" s="4" t="s">
         <v>664</v>
       </c>
-    </row>
-    <row r="197" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H196" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A197" s="5" t="s">
         <v>204</v>
       </c>
@@ -7173,8 +7765,11 @@
       <c r="G197" s="4" t="s">
         <v>665</v>
       </c>
-    </row>
-    <row r="198" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H197" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A198" s="7" t="s">
         <v>205</v>
       </c>
@@ -7196,8 +7791,11 @@
       <c r="G198" s="4" t="s">
         <v>666</v>
       </c>
-    </row>
-    <row r="199" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H198" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A199" s="5" t="s">
         <v>206</v>
       </c>
@@ -7214,13 +7812,16 @@
         <v>667</v>
       </c>
       <c r="F199" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="G199" s="4" t="s">
         <v>667</v>
       </c>
-    </row>
-    <row r="200" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H199" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A200" s="5" t="s">
         <v>207</v>
       </c>
@@ -7242,8 +7843,11 @@
       <c r="G200" s="4" t="s">
         <v>472</v>
       </c>
-    </row>
-    <row r="201" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H200" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A201" s="5" t="s">
         <v>208</v>
       </c>
@@ -7265,8 +7869,11 @@
       <c r="G201" s="4" t="s">
         <v>668</v>
       </c>
-    </row>
-    <row r="202" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H201" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A202" s="5" t="s">
         <v>209</v>
       </c>
@@ -7288,8 +7895,11 @@
       <c r="G202" s="4" t="s">
         <v>669</v>
       </c>
-    </row>
-    <row r="203" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H202" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A203" s="5" t="s">
         <v>210</v>
       </c>
@@ -7311,8 +7921,11 @@
       <c r="G203" s="4" t="s">
         <v>670</v>
       </c>
-    </row>
-    <row r="204" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H203" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A204" s="5" t="s">
         <v>211</v>
       </c>
@@ -7334,8 +7947,11 @@
       <c r="G204" s="4" t="s">
         <v>671</v>
       </c>
-    </row>
-    <row r="205" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H204" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A205" s="5" t="s">
         <v>212</v>
       </c>
@@ -7357,8 +7973,11 @@
       <c r="G205" s="4" t="s">
         <v>672</v>
       </c>
-    </row>
-    <row r="206" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H205" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="206" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A206" s="5" t="s">
         <v>213</v>
       </c>
@@ -7380,8 +7999,11 @@
       <c r="G206" s="4" t="s">
         <v>673</v>
       </c>
-    </row>
-    <row r="207" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H206" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A207" s="5" t="s">
         <v>214</v>
       </c>
@@ -7403,8 +8025,11 @@
       <c r="G207" s="4" t="s">
         <v>674</v>
       </c>
-    </row>
-    <row r="208" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H207" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A208" s="5" t="s">
         <v>215</v>
       </c>
@@ -7426,8 +8051,11 @@
       <c r="G208" s="4" t="s">
         <v>675</v>
       </c>
-    </row>
-    <row r="209" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H208" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A209" s="5" t="s">
         <v>216</v>
       </c>
@@ -7449,8 +8077,11 @@
       <c r="G209" s="4" t="s">
         <v>676</v>
       </c>
-    </row>
-    <row r="210" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H209" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="210" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A210" s="5" t="s">
         <v>217</v>
       </c>
@@ -7467,13 +8098,16 @@
         <v>677</v>
       </c>
       <c r="F210" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="G210" s="4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="211" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H210" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="211" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A211" s="5" t="s">
         <v>218</v>
       </c>
@@ -7495,8 +8129,11 @@
       <c r="G211" s="4" t="s">
         <v>678</v>
       </c>
-    </row>
-    <row r="212" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H211" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="212" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A212" s="7" t="s">
         <v>219</v>
       </c>
@@ -7518,8 +8155,11 @@
       <c r="G212" s="4" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="213" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H212" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="213" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A213" s="5" t="s">
         <v>220</v>
       </c>
@@ -7536,13 +8176,16 @@
         <v>680</v>
       </c>
       <c r="F213" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="G213" s="4" t="s">
         <v>680</v>
       </c>
-    </row>
-    <row r="214" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H213" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="214" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A214" s="5" t="s">
         <v>221</v>
       </c>
@@ -7564,8 +8207,11 @@
       <c r="G214" s="4" t="s">
         <v>681</v>
       </c>
-    </row>
-    <row r="215" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H214" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="215" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A215" s="5" t="s">
         <v>222</v>
       </c>
@@ -7587,8 +8233,11 @@
       <c r="G215" s="4" t="s">
         <v>682</v>
       </c>
-    </row>
-    <row r="216" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H215" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="216" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A216" s="5" t="s">
         <v>223</v>
       </c>
@@ -7610,8 +8259,11 @@
       <c r="G216" s="4" t="s">
         <v>683</v>
       </c>
-    </row>
-    <row r="217" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H216" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="217" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A217" s="5" t="s">
         <v>224</v>
       </c>
@@ -7633,8 +8285,11 @@
       <c r="G217" s="4" t="s">
         <v>684</v>
       </c>
-    </row>
-    <row r="218" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H217" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="218" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A218" s="5" t="s">
         <v>225</v>
       </c>
@@ -7656,8 +8311,11 @@
       <c r="G218" s="4" t="s">
         <v>685</v>
       </c>
-    </row>
-    <row r="219" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H218" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="219" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A219" s="5" t="s">
         <v>226</v>
       </c>
@@ -7679,8 +8337,11 @@
       <c r="G219" s="4" t="s">
         <v>686</v>
       </c>
-    </row>
-    <row r="220" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H219" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="220" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A220" s="5" t="s">
         <v>227</v>
       </c>
@@ -7702,8 +8363,11 @@
       <c r="G220" s="4" t="s">
         <v>687</v>
       </c>
-    </row>
-    <row r="221" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H220" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="221" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A221" s="5" t="s">
         <v>228</v>
       </c>
@@ -7725,8 +8389,11 @@
       <c r="G221" s="11" t="s">
         <v>688</v>
       </c>
-    </row>
-    <row r="222" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H221" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="222" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A222" s="5" t="s">
         <v>229</v>
       </c>
@@ -7748,8 +8415,11 @@
       <c r="G222" s="4" t="s">
         <v>689</v>
       </c>
-    </row>
-    <row r="223" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H222" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="223" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A223" s="5" t="s">
         <v>230</v>
       </c>
@@ -7771,8 +8441,11 @@
       <c r="G223" s="4" t="s">
         <v>690</v>
       </c>
-    </row>
-    <row r="224" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="H223" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="224" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A224" s="5" t="s">
         <v>231</v>
       </c>
@@ -7789,13 +8462,16 @@
         <v>691</v>
       </c>
       <c r="F224" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="G224" s="4" t="s">
         <v>691</v>
       </c>
-    </row>
-    <row r="225" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="H224" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="225" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A225" s="5" t="s">
         <v>232</v>
       </c>
@@ -7817,8 +8493,11 @@
       <c r="G225" s="4" t="s">
         <v>692</v>
       </c>
-    </row>
-    <row r="226" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="H225" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="226" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A226" s="7" t="s">
         <v>233</v>
       </c>
@@ -7840,11 +8519,20 @@
       <c r="G226" s="4" t="s">
         <v>693</v>
       </c>
-    </row>
-    <row r="227" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="H226" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="227" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="B227" s="6" t="s">
         <v>696</v>
       </c>
+      <c r="C227" t="s">
+        <v>700</v>
+      </c>
+      <c r="D227" s="4" t="s">
+        <v>700</v>
+      </c>
       <c r="E227" s="4" t="s">
         <v>697</v>
       </c>
@@ -7854,171 +8542,192 @@
       <c r="G227" s="4" t="s">
         <v>697</v>
       </c>
-      <c r="H227" t="s">
+      <c r="H227" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="228" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="B228" s="6" t="s">
+        <v>701</v>
+      </c>
+      <c r="C228" t="s">
+        <v>5</v>
+      </c>
+      <c r="D228" s="4" t="s">
+        <v>700</v>
+      </c>
+      <c r="E228" s="4" t="s">
         <v>702</v>
       </c>
-      <c r="I227" s="4" t="s">
+      <c r="F228" t="s">
+        <v>703</v>
+      </c>
+      <c r="G228" s="4" t="s">
         <v>702</v>
       </c>
-    </row>
-    <row r="228" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="B228" s="6" t="s">
+      <c r="H228" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="229" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B229" s="6" t="s">
+        <v>704</v>
+      </c>
+      <c r="C229" t="s">
+        <v>5</v>
+      </c>
+      <c r="D229" t="s">
+        <v>10</v>
+      </c>
+      <c r="E229" t="s">
+        <v>705</v>
+      </c>
+      <c r="F229" t="s">
         <v>703</v>
       </c>
-      <c r="E228" s="4" t="s">
-        <v>704</v>
-      </c>
-      <c r="F228" t="s">
+      <c r="G229" t="s">
         <v>705</v>
       </c>
-      <c r="G228" s="4" t="s">
-        <v>704</v>
-      </c>
-      <c r="H228" t="s">
+      <c r="H229" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="230" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="B230" s="6" t="s">
+        <v>706</v>
+      </c>
+      <c r="C230" t="s">
         <v>5</v>
       </c>
-      <c r="I228" s="4" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B229" s="6" t="s">
-        <v>706</v>
-      </c>
-      <c r="E229" t="s">
+      <c r="D230" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E230" s="4" t="s">
         <v>707</v>
       </c>
-      <c r="F229" t="s">
-        <v>705</v>
-      </c>
-      <c r="G229" t="s">
+      <c r="F230" t="s">
+        <v>703</v>
+      </c>
+      <c r="G230" s="4" t="s">
         <v>707</v>
       </c>
-      <c r="H229" t="s">
-        <v>5</v>
-      </c>
-      <c r="I229" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="230" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="B230" s="6" t="s">
+      <c r="H230" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="231" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="B231" s="6" t="s">
         <v>708</v>
       </c>
-      <c r="E230" s="4" t="s">
+      <c r="C231" t="s">
+        <v>52</v>
+      </c>
+      <c r="D231" s="4" t="s">
+        <v>700</v>
+      </c>
+      <c r="E231" s="4" t="s">
         <v>709</v>
       </c>
-      <c r="F230" t="s">
-        <v>705</v>
-      </c>
-      <c r="G230" s="4" t="s">
+      <c r="F231" t="s">
+        <v>703</v>
+      </c>
+      <c r="G231" t="s">
         <v>709</v>
       </c>
-      <c r="H230" t="s">
-        <v>5</v>
-      </c>
-      <c r="I230" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="231" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="B231" s="6" t="s">
+      <c r="H231" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="232" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="B232" s="6" t="s">
         <v>710</v>
       </c>
-      <c r="E231" s="4" t="s">
+      <c r="C232" t="s">
+        <v>67</v>
+      </c>
+      <c r="D232" s="4" t="s">
+        <v>700</v>
+      </c>
+      <c r="E232" s="4" t="s">
         <v>711</v>
       </c>
-      <c r="F231" t="s">
-        <v>705</v>
-      </c>
-      <c r="G231" t="s">
+      <c r="F232" t="s">
+        <v>703</v>
+      </c>
+      <c r="G232" s="4" t="s">
         <v>711</v>
       </c>
-      <c r="H231" t="s">
-        <v>52</v>
-      </c>
-      <c r="I231" s="4" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="232" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="B232" s="6" t="s">
+      <c r="H232" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="233" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="B233" s="6" t="s">
+        <v>714</v>
+      </c>
+      <c r="C233" t="s">
+        <v>82</v>
+      </c>
+      <c r="D233" s="4" t="s">
+        <v>700</v>
+      </c>
+      <c r="E233" s="4" t="s">
+        <v>715</v>
+      </c>
+      <c r="F233" t="s">
+        <v>703</v>
+      </c>
+      <c r="G233" t="s">
+        <v>715</v>
+      </c>
+      <c r="H233" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="234" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="B234" s="6" t="s">
+        <v>716</v>
+      </c>
+      <c r="C234" t="s">
         <v>712</v>
       </c>
-      <c r="E232" s="4" t="s">
-        <v>713</v>
-      </c>
-      <c r="F232" t="s">
-        <v>705</v>
-      </c>
-      <c r="G232" s="4" t="s">
-        <v>713</v>
-      </c>
-      <c r="H232" t="s">
-        <v>67</v>
-      </c>
-      <c r="I232" s="4" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="233" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="B233" s="6" t="s">
-        <v>716</v>
-      </c>
-      <c r="E233" s="4" t="s">
+      <c r="D234" s="4" t="s">
+        <v>700</v>
+      </c>
+      <c r="E234" s="4" t="s">
         <v>717</v>
       </c>
-      <c r="F233" t="s">
-        <v>705</v>
-      </c>
-      <c r="G233" t="s">
+      <c r="F234" t="s">
+        <v>703</v>
+      </c>
+      <c r="G234" s="4" t="s">
         <v>717</v>
       </c>
-      <c r="H233" t="s">
-        <v>82</v>
-      </c>
-      <c r="I233" s="4" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="234" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="B234" s="6" t="s">
+      <c r="H234" s="12" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="235" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="B235" s="6" t="s">
         <v>718</v>
       </c>
-      <c r="E234" s="4" t="s">
+      <c r="C235" t="s">
+        <v>126</v>
+      </c>
+      <c r="D235" s="4" t="s">
+        <v>700</v>
+      </c>
+      <c r="E235" s="4" t="s">
         <v>719</v>
       </c>
-      <c r="F234" t="s">
-        <v>705</v>
-      </c>
-      <c r="G234" s="4" t="s">
+      <c r="F235" t="s">
+        <v>703</v>
+      </c>
+      <c r="G235" t="s">
         <v>719</v>
       </c>
-      <c r="H234" t="s">
-        <v>714</v>
-      </c>
-      <c r="I234" s="4" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="235" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="B235" s="6" t="s">
-        <v>720</v>
-      </c>
-      <c r="E235" s="4" t="s">
-        <v>721</v>
-      </c>
-      <c r="F235" t="s">
-        <v>705</v>
-      </c>
-      <c r="G235" t="s">
-        <v>721</v>
-      </c>
-      <c r="H235" t="s">
-        <v>126</v>
-      </c>
-      <c r="I235" s="4" t="s">
-        <v>702</v>
+      <c r="H235" s="12" t="s">
+        <v>721</v>
       </c>
     </row>
   </sheetData>
@@ -8028,6 +8737,242 @@
   <conditionalFormatting sqref="G2">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="H3" r:id="rId2"/>
+    <hyperlink ref="H4" r:id="rId3"/>
+    <hyperlink ref="H6" r:id="rId4"/>
+    <hyperlink ref="H8" r:id="rId5"/>
+    <hyperlink ref="H10" r:id="rId6"/>
+    <hyperlink ref="H12" r:id="rId7"/>
+    <hyperlink ref="H14" r:id="rId8"/>
+    <hyperlink ref="H16" r:id="rId9"/>
+    <hyperlink ref="H18" r:id="rId10"/>
+    <hyperlink ref="H20" r:id="rId11"/>
+    <hyperlink ref="H22" r:id="rId12"/>
+    <hyperlink ref="H24" r:id="rId13"/>
+    <hyperlink ref="H26" r:id="rId14"/>
+    <hyperlink ref="H28" r:id="rId15"/>
+    <hyperlink ref="H30" r:id="rId16"/>
+    <hyperlink ref="H32" r:id="rId17"/>
+    <hyperlink ref="H34" r:id="rId18"/>
+    <hyperlink ref="H36" r:id="rId19"/>
+    <hyperlink ref="H38" r:id="rId20"/>
+    <hyperlink ref="H40" r:id="rId21"/>
+    <hyperlink ref="H42" r:id="rId22"/>
+    <hyperlink ref="H44" r:id="rId23"/>
+    <hyperlink ref="H46" r:id="rId24"/>
+    <hyperlink ref="H48" r:id="rId25"/>
+    <hyperlink ref="H50" r:id="rId26"/>
+    <hyperlink ref="H52" r:id="rId27"/>
+    <hyperlink ref="H54" r:id="rId28"/>
+    <hyperlink ref="H56" r:id="rId29"/>
+    <hyperlink ref="H58" r:id="rId30"/>
+    <hyperlink ref="H60" r:id="rId31"/>
+    <hyperlink ref="H62" r:id="rId32"/>
+    <hyperlink ref="H64" r:id="rId33"/>
+    <hyperlink ref="H66" r:id="rId34"/>
+    <hyperlink ref="H68" r:id="rId35"/>
+    <hyperlink ref="H70" r:id="rId36"/>
+    <hyperlink ref="H72" r:id="rId37"/>
+    <hyperlink ref="H74" r:id="rId38"/>
+    <hyperlink ref="H76" r:id="rId39"/>
+    <hyperlink ref="H78" r:id="rId40"/>
+    <hyperlink ref="H80" r:id="rId41"/>
+    <hyperlink ref="H82" r:id="rId42"/>
+    <hyperlink ref="H84" r:id="rId43"/>
+    <hyperlink ref="H86" r:id="rId44"/>
+    <hyperlink ref="H88" r:id="rId45"/>
+    <hyperlink ref="H90" r:id="rId46"/>
+    <hyperlink ref="H92" r:id="rId47"/>
+    <hyperlink ref="H94" r:id="rId48"/>
+    <hyperlink ref="H96" r:id="rId49"/>
+    <hyperlink ref="H98" r:id="rId50"/>
+    <hyperlink ref="H100" r:id="rId51"/>
+    <hyperlink ref="H102" r:id="rId52"/>
+    <hyperlink ref="H104" r:id="rId53"/>
+    <hyperlink ref="H106" r:id="rId54"/>
+    <hyperlink ref="H108" r:id="rId55"/>
+    <hyperlink ref="H110" r:id="rId56"/>
+    <hyperlink ref="H112" r:id="rId57"/>
+    <hyperlink ref="H114" r:id="rId58"/>
+    <hyperlink ref="H116" r:id="rId59"/>
+    <hyperlink ref="H118" r:id="rId60"/>
+    <hyperlink ref="H120" r:id="rId61"/>
+    <hyperlink ref="H122" r:id="rId62"/>
+    <hyperlink ref="H124" r:id="rId63"/>
+    <hyperlink ref="H126" r:id="rId64"/>
+    <hyperlink ref="H128" r:id="rId65"/>
+    <hyperlink ref="H130" r:id="rId66"/>
+    <hyperlink ref="H132" r:id="rId67"/>
+    <hyperlink ref="H134" r:id="rId68"/>
+    <hyperlink ref="H136" r:id="rId69"/>
+    <hyperlink ref="H138" r:id="rId70"/>
+    <hyperlink ref="H140" r:id="rId71"/>
+    <hyperlink ref="H142" r:id="rId72"/>
+    <hyperlink ref="H144" r:id="rId73"/>
+    <hyperlink ref="H146" r:id="rId74"/>
+    <hyperlink ref="H148" r:id="rId75"/>
+    <hyperlink ref="H150" r:id="rId76"/>
+    <hyperlink ref="H152" r:id="rId77"/>
+    <hyperlink ref="H154" r:id="rId78"/>
+    <hyperlink ref="H156" r:id="rId79"/>
+    <hyperlink ref="H158" r:id="rId80"/>
+    <hyperlink ref="H160" r:id="rId81"/>
+    <hyperlink ref="H162" r:id="rId82"/>
+    <hyperlink ref="H164" r:id="rId83"/>
+    <hyperlink ref="H166" r:id="rId84"/>
+    <hyperlink ref="H168" r:id="rId85"/>
+    <hyperlink ref="H170" r:id="rId86"/>
+    <hyperlink ref="H172" r:id="rId87"/>
+    <hyperlink ref="H174" r:id="rId88"/>
+    <hyperlink ref="H176" r:id="rId89"/>
+    <hyperlink ref="H178" r:id="rId90"/>
+    <hyperlink ref="H180" r:id="rId91"/>
+    <hyperlink ref="H182" r:id="rId92"/>
+    <hyperlink ref="H184" r:id="rId93"/>
+    <hyperlink ref="H186" r:id="rId94"/>
+    <hyperlink ref="H188" r:id="rId95"/>
+    <hyperlink ref="H190" r:id="rId96"/>
+    <hyperlink ref="H192" r:id="rId97"/>
+    <hyperlink ref="H194" r:id="rId98"/>
+    <hyperlink ref="H196" r:id="rId99"/>
+    <hyperlink ref="H198" r:id="rId100"/>
+    <hyperlink ref="H200" r:id="rId101"/>
+    <hyperlink ref="H202" r:id="rId102"/>
+    <hyperlink ref="H204" r:id="rId103"/>
+    <hyperlink ref="H206" r:id="rId104"/>
+    <hyperlink ref="H208" r:id="rId105"/>
+    <hyperlink ref="H210" r:id="rId106"/>
+    <hyperlink ref="H212" r:id="rId107"/>
+    <hyperlink ref="H214" r:id="rId108"/>
+    <hyperlink ref="H216" r:id="rId109"/>
+    <hyperlink ref="H218" r:id="rId110"/>
+    <hyperlink ref="H220" r:id="rId111"/>
+    <hyperlink ref="H222" r:id="rId112"/>
+    <hyperlink ref="H224" r:id="rId113"/>
+    <hyperlink ref="H226" r:id="rId114"/>
+    <hyperlink ref="H228" r:id="rId115"/>
+    <hyperlink ref="H230" r:id="rId116"/>
+    <hyperlink ref="H232" r:id="rId117"/>
+    <hyperlink ref="H234" r:id="rId118"/>
+    <hyperlink ref="H5" r:id="rId119"/>
+    <hyperlink ref="H7" r:id="rId120"/>
+    <hyperlink ref="H9" r:id="rId121"/>
+    <hyperlink ref="H11" r:id="rId122"/>
+    <hyperlink ref="H13" r:id="rId123"/>
+    <hyperlink ref="H15" r:id="rId124"/>
+    <hyperlink ref="H17" r:id="rId125"/>
+    <hyperlink ref="H19" r:id="rId126"/>
+    <hyperlink ref="H21" r:id="rId127"/>
+    <hyperlink ref="H23" r:id="rId128"/>
+    <hyperlink ref="H25" r:id="rId129"/>
+    <hyperlink ref="H27" r:id="rId130"/>
+    <hyperlink ref="H29" r:id="rId131"/>
+    <hyperlink ref="H31" r:id="rId132"/>
+    <hyperlink ref="H33" r:id="rId133"/>
+    <hyperlink ref="H35" r:id="rId134"/>
+    <hyperlink ref="H37" r:id="rId135"/>
+    <hyperlink ref="H39" r:id="rId136"/>
+    <hyperlink ref="H41" r:id="rId137"/>
+    <hyperlink ref="H43" r:id="rId138"/>
+    <hyperlink ref="H45" r:id="rId139"/>
+    <hyperlink ref="H47" r:id="rId140"/>
+    <hyperlink ref="H49" r:id="rId141"/>
+    <hyperlink ref="H51" r:id="rId142"/>
+    <hyperlink ref="H53" r:id="rId143"/>
+    <hyperlink ref="H55" r:id="rId144"/>
+    <hyperlink ref="H57" r:id="rId145"/>
+    <hyperlink ref="H59" r:id="rId146"/>
+    <hyperlink ref="H61" r:id="rId147"/>
+    <hyperlink ref="H63" r:id="rId148"/>
+    <hyperlink ref="H65" r:id="rId149"/>
+    <hyperlink ref="H67" r:id="rId150"/>
+    <hyperlink ref="H69" r:id="rId151"/>
+    <hyperlink ref="H71" r:id="rId152"/>
+    <hyperlink ref="H73" r:id="rId153"/>
+    <hyperlink ref="H75" r:id="rId154"/>
+    <hyperlink ref="H77" r:id="rId155"/>
+    <hyperlink ref="H79" r:id="rId156"/>
+    <hyperlink ref="H81" r:id="rId157"/>
+    <hyperlink ref="H83" r:id="rId158"/>
+    <hyperlink ref="H85" r:id="rId159"/>
+    <hyperlink ref="H87" r:id="rId160"/>
+    <hyperlink ref="H89" r:id="rId161"/>
+    <hyperlink ref="H91" r:id="rId162"/>
+    <hyperlink ref="H93" r:id="rId163"/>
+    <hyperlink ref="H95" r:id="rId164"/>
+    <hyperlink ref="H97" r:id="rId165"/>
+    <hyperlink ref="H99" r:id="rId166"/>
+    <hyperlink ref="H101" r:id="rId167"/>
+    <hyperlink ref="H103" r:id="rId168"/>
+    <hyperlink ref="H105" r:id="rId169"/>
+    <hyperlink ref="H107" r:id="rId170"/>
+    <hyperlink ref="H109" r:id="rId171"/>
+    <hyperlink ref="H111" r:id="rId172"/>
+    <hyperlink ref="H113" r:id="rId173"/>
+    <hyperlink ref="H115" r:id="rId174"/>
+    <hyperlink ref="H117" r:id="rId175"/>
+    <hyperlink ref="H119" r:id="rId176"/>
+    <hyperlink ref="H121" r:id="rId177"/>
+    <hyperlink ref="H123" r:id="rId178"/>
+    <hyperlink ref="H125" r:id="rId179"/>
+    <hyperlink ref="H127" r:id="rId180"/>
+    <hyperlink ref="H129" r:id="rId181"/>
+    <hyperlink ref="H131" r:id="rId182"/>
+    <hyperlink ref="H133" r:id="rId183"/>
+    <hyperlink ref="H135" r:id="rId184"/>
+    <hyperlink ref="H137" r:id="rId185"/>
+    <hyperlink ref="H139" r:id="rId186"/>
+    <hyperlink ref="H141" r:id="rId187"/>
+    <hyperlink ref="H143" r:id="rId188"/>
+    <hyperlink ref="H145" r:id="rId189"/>
+    <hyperlink ref="H147" r:id="rId190"/>
+    <hyperlink ref="H149" r:id="rId191"/>
+    <hyperlink ref="H151" r:id="rId192"/>
+    <hyperlink ref="H153" r:id="rId193"/>
+    <hyperlink ref="H155" r:id="rId194"/>
+    <hyperlink ref="H157" r:id="rId195"/>
+    <hyperlink ref="H159" r:id="rId196"/>
+    <hyperlink ref="H161" r:id="rId197"/>
+    <hyperlink ref="H163" r:id="rId198"/>
+    <hyperlink ref="H165" r:id="rId199"/>
+    <hyperlink ref="H167" r:id="rId200"/>
+    <hyperlink ref="H169" r:id="rId201"/>
+    <hyperlink ref="H171" r:id="rId202"/>
+    <hyperlink ref="H173" r:id="rId203"/>
+    <hyperlink ref="H175" r:id="rId204"/>
+    <hyperlink ref="H177" r:id="rId205"/>
+    <hyperlink ref="H179" r:id="rId206"/>
+    <hyperlink ref="H181" r:id="rId207"/>
+    <hyperlink ref="H183" r:id="rId208"/>
+    <hyperlink ref="H185" r:id="rId209"/>
+    <hyperlink ref="H187" r:id="rId210"/>
+    <hyperlink ref="H189" r:id="rId211"/>
+    <hyperlink ref="H191" r:id="rId212"/>
+    <hyperlink ref="H193" r:id="rId213"/>
+    <hyperlink ref="H195" r:id="rId214"/>
+    <hyperlink ref="H197" r:id="rId215"/>
+    <hyperlink ref="H199" r:id="rId216"/>
+    <hyperlink ref="H201" r:id="rId217"/>
+    <hyperlink ref="H203" r:id="rId218"/>
+    <hyperlink ref="H205" r:id="rId219"/>
+    <hyperlink ref="H207" r:id="rId220"/>
+    <hyperlink ref="H209" r:id="rId221"/>
+    <hyperlink ref="H211" r:id="rId222"/>
+    <hyperlink ref="H213" r:id="rId223"/>
+    <hyperlink ref="H215" r:id="rId224"/>
+    <hyperlink ref="H217" r:id="rId225"/>
+    <hyperlink ref="H219" r:id="rId226"/>
+    <hyperlink ref="H221" r:id="rId227"/>
+    <hyperlink ref="H223" r:id="rId228"/>
+    <hyperlink ref="H225" r:id="rId229"/>
+    <hyperlink ref="H227" r:id="rId230"/>
+    <hyperlink ref="H229" r:id="rId231"/>
+    <hyperlink ref="H231" r:id="rId232"/>
+    <hyperlink ref="H233" r:id="rId233"/>
+    <hyperlink ref="H235" r:id="rId234"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>